<commit_message>
material properties files for lit and he
</commit_message>
<xml_diff>
--- a/scripts/helium-properties-300-900C.xlsx
+++ b/scripts/helium-properties-300-900C.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\vanlew-ucla-phd-dissertation\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon\Documents\GitHub\vanlew-ucla-phd-dissertation\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="fluid" localSheetId="5">Sheet1!$A$1:$K$12</definedName>
+    <definedName name="fluid" localSheetId="5">Sheet1!$A$1:$M$12</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Temperature (C)</t>
   </si>
@@ -100,11 +100,30 @@
   <si>
     <t>average</t>
   </si>
+  <si>
+    <t>Scaled density</t>
+  </si>
+  <si>
+    <t>Scaled kinematic viscosity</t>
+  </si>
+  <si>
+    <t>Scaled diffusivity</t>
+  </si>
+  <si>
+    <t>Scaled conductivity</t>
+  </si>
+  <si>
+    <t>Scaled viscosity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,9 +153,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -194,7 +215,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -400,11 +420,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="385173504"/>
-        <c:axId val="385167520"/>
+        <c:axId val="74391680"/>
+        <c:axId val="74392240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="385173504"/>
+        <c:axId val="74391680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -461,12 +481,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385167520"/>
+        <c:crossAx val="74392240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="385167520"/>
+        <c:axId val="74392240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -523,7 +543,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385173504"/>
+        <c:crossAx val="74391680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -612,7 +632,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -767,7 +786,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$12</c:f>
+              <c:f>Sheet1!$K$2:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -817,11 +836,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="385170784"/>
-        <c:axId val="385170240"/>
+        <c:axId val="176356016"/>
+        <c:axId val="176356576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="385170784"/>
+        <c:axId val="176356016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -878,12 +897,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385170240"/>
+        <c:crossAx val="176356576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="385170240"/>
+        <c:axId val="176356576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -940,7 +959,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385170784"/>
+        <c:crossAx val="176356016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1028,7 +1047,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1133,7 +1151,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$12</c:f>
+              <c:f>Sheet1!$Q$2:$Q$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1183,11 +1201,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="385179488"/>
-        <c:axId val="385180032"/>
+        <c:axId val="176358816"/>
+        <c:axId val="176359376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="385179488"/>
+        <c:axId val="176358816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1244,12 +1262,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385180032"/>
+        <c:crossAx val="176359376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="385180032"/>
+        <c:axId val="176359376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1306,7 +1324,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385179488"/>
+        <c:crossAx val="176358816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1500,7 +1518,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$2:$L$12</c:f>
+              <c:f>Sheet1!$O$2:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1550,11 +1568,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="385169696"/>
-        <c:axId val="385168064"/>
+        <c:axId val="176361616"/>
+        <c:axId val="176362176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="385169696"/>
+        <c:axId val="176361616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1611,12 +1629,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385168064"/>
+        <c:crossAx val="176362176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="385168064"/>
+        <c:axId val="176362176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1673,7 +1691,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385169696"/>
+        <c:crossAx val="176361616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1887,7 +1905,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$12</c:f>
+              <c:f>Sheet1!$M$2:$M$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1937,11 +1955,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="385177856"/>
-        <c:axId val="284107872"/>
+        <c:axId val="176592368"/>
+        <c:axId val="176592928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="385177856"/>
+        <c:axId val="176592368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1998,12 +2016,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="284107872"/>
+        <c:crossAx val="176592928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="284107872"/>
+        <c:axId val="176592928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2060,7 +2078,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385177856"/>
+        <c:crossAx val="176592368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4888,7 +4906,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="93" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4899,7 +4917,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="93" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4910,7 +4928,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="93" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4921,7 +4939,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="93" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4932,7 +4950,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="93" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4943,7 +4961,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663609" cy="6286500"/>
+    <xdr:ext cx="8664677" cy="6288548"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -4970,7 +4988,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663609" cy="6286500"/>
+    <xdr:ext cx="8664677" cy="6288548"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -4997,7 +5015,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663609" cy="6286500"/>
+    <xdr:ext cx="8664677" cy="6288548"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -5024,7 +5042,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663609" cy="6286500"/>
+    <xdr:ext cx="8664677" cy="6288548"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -5051,7 +5069,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663609" cy="6286500"/>
+    <xdr:ext cx="8664677" cy="6288548"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -5341,10 +5359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5352,19 +5370,23 @@
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5375,37 +5397,52 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>400</v>
       </c>
@@ -5416,39 +5453,59 @@
         <v>7.1502999999999997E-2</v>
       </c>
       <c r="D2">
+        <f>C2/$C$2</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>13.984999999999999</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2102.6999999999998</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>3501.2</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>32.222999999999999</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>5.1929999999999996</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>1526.8</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>3.4921E-5</v>
       </c>
-      <c r="K2">
+      <c r="L2" s="1">
+        <f>K2/$K$2</f>
+        <v>1</v>
+      </c>
+      <c r="M2">
         <v>0.27348</v>
       </c>
-      <c r="L2" s="1">
-        <f>J2/C2</f>
+      <c r="N2">
+        <f>M2/$M$2</f>
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
+        <f t="shared" ref="O2:O12" si="0">K2/C2</f>
         <v>4.8838510272296266E-4</v>
       </c>
-      <c r="M2" s="1">
-        <f>K2/(C2*H2*1000)</f>
+      <c r="P2" s="1">
+        <f>O2/$O$2</f>
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1">
+        <f t="shared" ref="Q2:Q12" si="1">M2/(C2*I2*1000)</f>
         <v>7.365173553859364E-4</v>
       </c>
+      <c r="R2" s="1">
+        <f>Q2/$Q$2</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>450</v>
       </c>
@@ -5459,39 +5516,59 @@
         <v>6.6559999999999994E-2</v>
       </c>
       <c r="D3">
+        <f t="shared" ref="D3:D12" si="2">C3/$C$2</f>
+        <v>0.93087003342517094</v>
+      </c>
+      <c r="E3">
         <v>15.023999999999999</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2258.5</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>3760.9</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>32.595999999999997</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>5.1929999999999996</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>1582.5</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>3.6724000000000003E-5</v>
       </c>
-      <c r="K3">
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L12" si="3">K3/$K$2</f>
+        <v>1.0516308238595689</v>
+      </c>
+      <c r="M3">
         <v>0.28750999999999999</v>
       </c>
-      <c r="L3" s="1">
-        <f>J3/C3</f>
+      <c r="N3">
+        <f t="shared" ref="N3:N12" si="4">M3/$M$2</f>
+        <v>1.051301740529472</v>
+      </c>
+      <c r="O3" s="1">
+        <f t="shared" si="0"/>
         <v>5.517427884615386E-4</v>
       </c>
-      <c r="M3" s="1">
-        <f>K3/(C3*H3*1000)</f>
+      <c r="P3" s="1">
+        <f t="shared" ref="P3:P12" si="5">O3/$O$2</f>
+        <v>1.1297289482937314</v>
+      </c>
+      <c r="Q3" s="1">
+        <f t="shared" si="1"/>
         <v>8.3180460197899541E-4</v>
       </c>
+      <c r="R3" s="1">
+        <f t="shared" ref="R3:R12" si="6">Q3/$Q$2</f>
+        <v>1.1293754259777466</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>500</v>
       </c>
@@ -5502,39 +5579,59 @@
         <v>6.2257E-2</v>
       </c>
       <c r="D4">
+        <f t="shared" si="2"/>
+        <v>0.87069074024866089</v>
+      </c>
+      <c r="E4">
         <v>16.062999999999999</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2414.3000000000002</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>4020.5</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>32.942999999999998</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>5.1929999999999996</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1636.3</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>3.8494000000000001E-5</v>
       </c>
-      <c r="K4">
+      <c r="L4" s="1">
+        <f t="shared" si="3"/>
+        <v>1.1023166575985797</v>
+      </c>
+      <c r="M4">
         <v>0.30125000000000002</v>
       </c>
-      <c r="L4" s="1">
-        <f>J4/C4</f>
+      <c r="N4">
+        <f t="shared" si="4"/>
+        <v>1.1015430744478574</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" si="0"/>
         <v>6.1830798143180693E-4</v>
       </c>
-      <c r="M4" s="1">
-        <f>K4/(C4*H4*1000)</f>
+      <c r="P4" s="1">
+        <f t="shared" si="5"/>
+        <v>1.2660254745373412</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" si="1"/>
         <v>9.3179536031855398E-4</v>
       </c>
+      <c r="R4" s="1">
+        <f t="shared" si="6"/>
+        <v>1.265137003907113</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>550</v>
       </c>
@@ -5545,39 +5642,59 @@
         <v>5.8476E-2</v>
       </c>
       <c r="D5">
+        <f t="shared" si="2"/>
+        <v>0.81781184006265473</v>
+      </c>
+      <c r="E5">
         <v>17.100999999999999</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>2570.1</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>4280.2</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>33.268000000000001</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>5.1929999999999996</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>1688.3</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>4.0231000000000002E-5</v>
       </c>
-      <c r="K5">
+      <c r="L5" s="1">
+        <f t="shared" si="3"/>
+        <v>1.1520575012170329</v>
+      </c>
+      <c r="M5">
         <v>0.31473000000000001</v>
       </c>
-      <c r="L5" s="1">
-        <f>J5/C5</f>
+      <c r="N5">
+        <f t="shared" si="4"/>
+        <v>1.1508336989907855</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="0"/>
         <v>6.8799165469594361E-4</v>
       </c>
-      <c r="M5" s="1">
-        <f>K5/(C5*H5*1000)</f>
+      <c r="P5" s="1">
+        <f t="shared" si="5"/>
+        <v>1.4087072903331537</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" si="1"/>
         <v>1.0364352176715495E-3</v>
       </c>
+      <c r="R5" s="1">
+        <f t="shared" si="6"/>
+        <v>1.4072108553755065</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>600</v>
       </c>
@@ -5588,39 +5705,59 @@
         <v>5.5128000000000003E-2</v>
       </c>
       <c r="D6">
+        <f t="shared" si="2"/>
+        <v>0.77098862984769878</v>
+      </c>
+      <c r="E6">
         <v>18.14</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>2725.8</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>4539.8</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>33.573999999999998</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>5.1929999999999996</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>1738.9</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>4.1940000000000002E-5</v>
       </c>
-      <c r="K6">
+      <c r="L6" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2009965350362246</v>
+      </c>
+      <c r="M6">
         <v>0.32796999999999998</v>
       </c>
-      <c r="L6" s="1">
-        <f>J6/C6</f>
+      <c r="N6">
+        <f t="shared" si="4"/>
+        <v>1.1992467456486762</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="0"/>
         <v>7.6077492381366996E-4</v>
       </c>
-      <c r="M6" s="1">
-        <f>K6/(C6*H6*1000)</f>
+      <c r="P6" s="1">
+        <f t="shared" si="5"/>
+        <v>1.5577357285716</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" si="1"/>
         <v>1.145627843739841E-3</v>
       </c>
+      <c r="R6" s="1">
+        <f t="shared" si="6"/>
+        <v>1.5554661887628296</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>650</v>
       </c>
@@ -5631,39 +5768,59 @@
         <v>5.2142000000000001E-2</v>
       </c>
       <c r="D7">
+        <f t="shared" si="2"/>
+        <v>0.72922814427366689</v>
+      </c>
+      <c r="E7">
         <v>19.178000000000001</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>2881.6</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>4799.5</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>33.863999999999997</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>5.1929999999999996</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>1787.9</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>4.3621999999999997E-5</v>
       </c>
-      <c r="K7">
+      <c r="L7" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2491623951204145</v>
+      </c>
+      <c r="M7">
         <v>0.34099000000000002</v>
       </c>
-      <c r="L7" s="1">
-        <f>J7/C7</f>
+      <c r="N7">
+        <f t="shared" si="4"/>
+        <v>1.2468553459119498</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="0"/>
         <v>8.3660005369951278E-4</v>
       </c>
-      <c r="M7" s="1">
-        <f>K7/(C7*H7*1000)</f>
+      <c r="P7" s="1">
+        <f t="shared" si="5"/>
+        <v>1.7129925729411031</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" si="1"/>
         <v>1.2593186496313452E-3</v>
       </c>
+      <c r="R7" s="1">
+        <f t="shared" si="6"/>
+        <v>1.7098288864781197</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>700</v>
       </c>
@@ -5674,39 +5831,59 @@
         <v>4.9464000000000001E-2</v>
       </c>
       <c r="D8">
+        <f t="shared" si="2"/>
+        <v>0.69177517027257607</v>
+      </c>
+      <c r="E8">
         <v>20.216999999999999</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>3037.4</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>5059.1000000000004</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>34.137</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>5.1929999999999996</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>1835.7</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>4.528E-5</v>
       </c>
-      <c r="K8">
+      <c r="L8" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2966409896623807</v>
+      </c>
+      <c r="M8">
         <v>0.3538</v>
       </c>
-      <c r="L8" s="1">
-        <f>J8/C8</f>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>1.2936960655258154</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="0"/>
         <v>9.1541322982371021E-4</v>
       </c>
-      <c r="M8" s="1">
-        <f>K8/(C8*H8*1000)</f>
+      <c r="P8" s="1">
+        <f t="shared" si="5"/>
+        <v>1.8743676347207914</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" si="1"/>
         <v>1.377368899318585E-3</v>
       </c>
+      <c r="R8" s="1">
+        <f t="shared" si="6"/>
+        <v>1.870110580893021</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>750</v>
       </c>
@@ -5717,39 +5894,59 @@
         <v>4.7046999999999999E-2</v>
       </c>
       <c r="D9">
+        <f t="shared" si="2"/>
+        <v>0.65797239276673702</v>
+      </c>
+      <c r="E9">
         <v>21.254999999999999</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>3193.2</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>5318.8</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>34.398000000000003</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>5.1929999999999996</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>1882.3</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>4.6913000000000003E-5</v>
       </c>
-      <c r="K9">
+      <c r="L9" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3434036825978639</v>
+      </c>
+      <c r="M9">
         <v>0.36642000000000002</v>
       </c>
-      <c r="L9" s="1">
-        <f>J9/C9</f>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>1.3398420359806933</v>
+      </c>
+      <c r="O9" s="1">
+        <f t="shared" si="0"/>
         <v>9.9715178438582706E-4</v>
       </c>
-      <c r="M9" s="1">
-        <f>K9/(C9*H9*1000)</f>
+      <c r="P9" s="1">
+        <f t="shared" si="5"/>
+        <v>2.0417325975470288</v>
+      </c>
+      <c r="Q9" s="1">
+        <f t="shared" si="1"/>
         <v>1.4997846776304688E-3</v>
       </c>
+      <c r="R9" s="1">
+        <f t="shared" si="6"/>
+        <v>2.0363195336307847</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>800</v>
       </c>
@@ -5760,39 +5957,59 @@
         <v>4.4854999999999999E-2</v>
       </c>
       <c r="D10">
+        <f t="shared" si="2"/>
+        <v>0.62731633637749462</v>
+      </c>
+      <c r="E10">
         <v>22.294</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>3349</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>5578.4</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>34.645000000000003</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>5.1929999999999996</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>1927.7</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>4.8525E-5</v>
       </c>
-      <c r="K10">
+      <c r="L10" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3895650181839008</v>
+      </c>
+      <c r="M10">
         <v>0.37885999999999997</v>
       </c>
-      <c r="L10" s="1">
-        <f>J10/C10</f>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>1.3853298230217932</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="0"/>
         <v>1.0818191951844833E-3</v>
       </c>
-      <c r="M10" s="1">
-        <f>K10/(C10*H10*1000)</f>
+      <c r="P10" s="1">
+        <f t="shared" si="5"/>
+        <v>2.2150945824368176</v>
+      </c>
+      <c r="Q10" s="1">
+        <f t="shared" si="1"/>
         <v>1.6264831607625942E-3</v>
       </c>
+      <c r="R10" s="1">
+        <f t="shared" si="6"/>
+        <v>2.2083432913951011</v>
+      </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>850</v>
       </c>
@@ -5803,39 +6020,59 @@
         <v>4.2858E-2</v>
       </c>
       <c r="D11">
+        <f t="shared" si="2"/>
+        <v>0.59938743828930252</v>
+      </c>
+      <c r="E11">
         <v>23.332999999999998</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>3504.8</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>5838.1</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>34.881999999999998</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>5.1929999999999996</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>1972.1</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>5.0115999999999999E-5</v>
       </c>
-      <c r="K11">
+      <c r="L11" s="1">
+        <f t="shared" si="3"/>
+        <v>1.435124996420492</v>
+      </c>
+      <c r="M11">
         <v>0.39112999999999998</v>
       </c>
-      <c r="L11" s="1">
-        <f>J11/C11</f>
+      <c r="N11">
+        <f t="shared" si="4"/>
+        <v>1.4301959923943248</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="0"/>
         <v>1.1693499463344065E-3</v>
       </c>
-      <c r="M11" s="1">
-        <f>K11/(C11*H11*1000)</f>
+      <c r="P11" s="1">
+        <f t="shared" si="5"/>
+        <v>2.3943194413891091</v>
+      </c>
+      <c r="Q11" s="1">
+        <f t="shared" si="1"/>
         <v>1.7574011444220696E-3</v>
       </c>
+      <c r="R11" s="1">
+        <f t="shared" si="6"/>
+        <v>2.386096039109884</v>
+      </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>900</v>
       </c>
@@ -5846,48 +6083,77 @@
         <v>4.1031999999999999E-2</v>
       </c>
       <c r="D12">
+        <f t="shared" si="2"/>
+        <v>0.57385004824972374</v>
+      </c>
+      <c r="E12">
         <v>24.370999999999999</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>3660.6</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>6097.7</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>35.107999999999997</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>5.1929999999999996</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>2015.5</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K12" s="1">
         <v>5.1687999999999997E-5</v>
       </c>
-      <c r="K12">
+      <c r="L12" s="1">
+        <f t="shared" si="3"/>
+        <v>1.4801408894361558</v>
+      </c>
+      <c r="M12">
         <v>0.40323999999999999</v>
       </c>
-      <c r="L12" s="1">
-        <f>J12/C12</f>
+      <c r="N12">
+        <f t="shared" si="4"/>
+        <v>1.4744771098434986</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="0"/>
         <v>1.2596997465392863E-3</v>
       </c>
-      <c r="M12" s="1">
-        <f>K12/(C12*H12*1000)</f>
+      <c r="P12" s="1">
+        <f t="shared" si="5"/>
+        <v>2.579316485117797</v>
+      </c>
+      <c r="Q12" s="1">
+        <f t="shared" si="1"/>
         <v>1.8924420845329343E-3</v>
       </c>
+      <c r="R12" s="1">
+        <f t="shared" si="6"/>
+        <v>2.5694466949000696</v>
+      </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L13" s="1">
-        <f>AVERAGE(L2:L12)</f>
-        <v>8.5156694609937712E-4</v>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C13" s="1">
+        <f>AVERAGE(C2:C12)</f>
+        <v>5.3756545454545453E-2</v>
       </c>
       <c r="M13" s="1">
         <f>AVERAGE(M2:M12)</f>
+        <v>0.33994363636363639</v>
+      </c>
+      <c r="O13" s="3">
+        <f>AVERAGE(O2:O12)</f>
+        <v>8.5156694609937712E-4</v>
+      </c>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="2">
+        <f>AVERAGE(Q2:Q12)</f>
         <v>1.2813617268538976E-3</v>
       </c>
-      <c r="N13" t="s">
+      <c r="R13" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tries to make intro better
</commit_message>
<xml_diff>
--- a/scripts/helium-properties-300-900C.xlsx
+++ b/scripts/helium-properties-300-900C.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon\Documents\GitHub\vanlew-ucla-phd-dissertation\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\GitHub\vanlew-ucla-phd-dissertation\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Temperature (C)</t>
   </si>
@@ -420,11 +420,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="74391680"/>
-        <c:axId val="74392240"/>
+        <c:axId val="1435128624"/>
+        <c:axId val="1435126992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74391680"/>
+        <c:axId val="1435128624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -481,12 +481,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74392240"/>
+        <c:crossAx val="1435126992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74392240"/>
+        <c:axId val="1435126992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -543,7 +543,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74391680"/>
+        <c:crossAx val="1435128624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -836,11 +836,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="176356016"/>
-        <c:axId val="176356576"/>
+        <c:axId val="1435129712"/>
+        <c:axId val="1435125904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="176356016"/>
+        <c:axId val="1435129712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -897,12 +897,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176356576"/>
+        <c:crossAx val="1435125904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="176356576"/>
+        <c:axId val="1435125904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -959,7 +959,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176356016"/>
+        <c:crossAx val="1435129712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1201,11 +1201,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="176358816"/>
-        <c:axId val="176359376"/>
+        <c:axId val="1435126448"/>
+        <c:axId val="1435130256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="176358816"/>
+        <c:axId val="1435126448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1262,12 +1262,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176359376"/>
+        <c:crossAx val="1435130256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="176359376"/>
+        <c:axId val="1435130256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1324,7 +1324,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176358816"/>
+        <c:crossAx val="1435126448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1413,7 +1413,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1568,11 +1567,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="176361616"/>
-        <c:axId val="176362176"/>
+        <c:axId val="1435133520"/>
+        <c:axId val="1435134608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="176361616"/>
+        <c:axId val="1435133520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1629,12 +1628,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176362176"/>
+        <c:crossAx val="1435134608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="176362176"/>
+        <c:axId val="1435134608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1691,7 +1690,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176361616"/>
+        <c:crossAx val="1435133520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1750,7 +1749,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1955,11 +1953,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="176592368"/>
-        <c:axId val="176592928"/>
+        <c:axId val="1435131888"/>
+        <c:axId val="1435122640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="176592368"/>
+        <c:axId val="1435131888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2016,12 +2014,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176592928"/>
+        <c:crossAx val="1435122640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="176592928"/>
+        <c:axId val="1435122640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2078,7 +2076,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176592368"/>
+        <c:crossAx val="1435131888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5359,10 +5357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5384,9 +5382,11 @@
     <col min="15" max="15" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.42578125" customWidth="1"/>
     <col min="17" max="17" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5441,8 +5441,11 @@
       <c r="R1" t="s">
         <v>16</v>
       </c>
+      <c r="S1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>400</v>
       </c>
@@ -5504,8 +5507,11 @@
         <f>Q2/$Q$2</f>
         <v>1</v>
       </c>
+      <c r="S2">
+        <v>1526.8</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>450</v>
       </c>
@@ -5567,8 +5573,11 @@
         <f t="shared" ref="R3:R12" si="6">Q3/$Q$2</f>
         <v>1.1293754259777466</v>
       </c>
+      <c r="S3">
+        <v>1582.5</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>500</v>
       </c>
@@ -5630,8 +5639,11 @@
         <f t="shared" si="6"/>
         <v>1.265137003907113</v>
       </c>
+      <c r="S4">
+        <v>1636.3</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>550</v>
       </c>
@@ -5693,8 +5705,11 @@
         <f t="shared" si="6"/>
         <v>1.4072108553755065</v>
       </c>
+      <c r="S5">
+        <v>1688.3</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>600</v>
       </c>
@@ -5756,8 +5771,11 @@
         <f t="shared" si="6"/>
         <v>1.5554661887628296</v>
       </c>
+      <c r="S6">
+        <v>1738.9</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>650</v>
       </c>
@@ -5819,8 +5837,11 @@
         <f t="shared" si="6"/>
         <v>1.7098288864781197</v>
       </c>
+      <c r="S7">
+        <v>1787.9</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>700</v>
       </c>
@@ -5882,8 +5903,11 @@
         <f t="shared" si="6"/>
         <v>1.870110580893021</v>
       </c>
+      <c r="S8">
+        <v>1835.7</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>750</v>
       </c>
@@ -5945,8 +5969,11 @@
         <f t="shared" si="6"/>
         <v>2.0363195336307847</v>
       </c>
+      <c r="S9">
+        <v>1882.3</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>800</v>
       </c>
@@ -6008,8 +6035,11 @@
         <f t="shared" si="6"/>
         <v>2.2083432913951011</v>
       </c>
+      <c r="S10">
+        <v>1927.7</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>850</v>
       </c>
@@ -6071,8 +6101,11 @@
         <f t="shared" si="6"/>
         <v>2.386096039109884</v>
       </c>
+      <c r="S11">
+        <v>1972.1</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>900</v>
       </c>
@@ -6134,8 +6167,11 @@
         <f t="shared" si="6"/>
         <v>2.5694466949000696</v>
       </c>
+      <c r="S12">
+        <v>2015.5</v>
+      </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
         <f>AVERAGE(C2:C12)</f>
         <v>5.3756545454545453E-2</v>

</xml_diff>